<commit_message>
added a Revenue field to the LoadExploreClean file
</commit_message>
<xml_diff>
--- a/data/RetailAnalysis.xlsx
+++ b/data/RetailAnalysis.xlsx
@@ -1,41 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/123fc4457e0ed43e/Desktop/python/datasets/Online Retail/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_7CF3FF633109AE413C978693B2725FDA7C6BC482" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{259E8701-CAE4-4FE3-B2AD-18D8392393F8}"/>
   <bookViews>
-    <workbookView xWindow="26985" yWindow="2070" windowWidth="30600" windowHeight="18945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Top Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Sales Trends" sheetId="2" r:id="rId2"/>
     <sheet name="Top Ten Products" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Ranking</t>
   </si>
@@ -188,31 +169,16 @@
   </si>
   <si>
     <t>PACK OF 72 RETRO SPOT CAKE CASES</t>
-  </si>
-  <si>
-    <t>Percent sales for top 10 customers</t>
-  </si>
-  <si>
-    <t>Total Sales Quantity for the timespan</t>
-  </si>
-  <si>
-    <t>Sales Quantity Percent by Product</t>
-  </si>
-  <si>
-    <t>Total Sales Quantity for the Timespan</t>
-  </si>
-  <si>
-    <t>Sales for Top Product by Quantity</t>
-  </si>
-  <si>
-    <t>Percent Sales by Quantity for Top Customer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +194,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -244,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -267,46 +226,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -327,13 +262,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenCustomers_chart.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenCustomers_chart.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -376,13 +305,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="MonthlySales_chart.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="MonthlySalesRevenue_chart.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -395,7 +318,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2600325" y="190500"/>
+          <a:off x="3286125" y="190500"/>
           <a:ext cx="10972822" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -425,13 +348,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenProductsSold_chart.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenProductsSold_chart.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -458,9 +375,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -498,7 +415,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -532,7 +449,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -567,10 +483,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -743,21 +658,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -768,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -779,7 +692,7 @@
         <v>365220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -790,7 +703,7 @@
         <v>281535</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -801,7 +714,7 @@
         <v>218090</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -812,7 +725,7 @@
         <v>186910</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -823,7 +736,7 @@
         <v>185538</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -834,7 +747,7 @@
         <v>176000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -845,7 +758,7 @@
         <v>163791</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -856,7 +769,7 @@
         <v>143727</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -867,7 +780,7 @@
         <v>117913</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -876,47 +789,6 @@
       </c>
       <c r="C11" s="1">
         <v>101095</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4">
-        <f>SUM(C2:C11)</f>
-        <v>1939819</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f>'Sales Trends'!B27</f>
-        <v>11635971</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <f>C12/A15</f>
-        <v>0.16670882043277693</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <f>C2/A15</f>
-        <v>3.1387152821195585E-2</v>
       </c>
     </row>
   </sheetData>
@@ -926,20 +798,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -947,211 +817,204 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>444339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>796632.9400000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1">
-        <v>395203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>622354.2120000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1">
-        <v>391853</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>531206.956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1">
-        <v>530301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>763112.071</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1">
-        <v>385569</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>587691.032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>423966</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>613172.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1">
-        <v>413695</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>676873.6899999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>358554</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>573146.9300000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="1">
-        <v>521757</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>654749.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1">
-        <v>592590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>850905.241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="1">
-        <v>622253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1041505.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>730369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1416320.112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1">
-        <v>542655</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1121929.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1">
-        <v>397004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>558368.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>286033</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>496775.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1">
-        <v>383893</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>681318.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
-        <v>311238</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>491919.041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1">
-        <v>398479</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>720972.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="1">
-        <v>393516</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>689391.15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1">
-        <v>405218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>678964.781</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="1">
-        <v>424266</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>681386.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="1">
-        <v>574063</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1017398.282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="1">
-        <v>626342</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1069265.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="1">
-        <v>768400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1456089.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="1">
-        <v>314415</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4">
-        <f>SUM(B2:B26)</f>
-        <v>11635971</v>
+        <v>432699.16</v>
       </c>
     </row>
   </sheetData>
@@ -1161,21 +1024,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1047,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1197,7 +1058,7 @@
         <v>108305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1208,7 +1069,7 @@
         <v>92926</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1219,7 +1080,7 @@
         <v>81087</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1230,7 +1091,7 @@
         <v>77905</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1241,7 +1102,7 @@
         <v>70664</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1252,7 +1113,7 @@
         <v>56399</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1263,7 +1124,7 @@
         <v>54187</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1274,7 +1135,7 @@
         <v>49577</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1285,7 +1146,7 @@
         <v>49283</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1294,47 +1155,6 @@
       </c>
       <c r="C11" s="1">
         <v>46055</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4">
-        <f>SUM(C2:C11)</f>
-        <v>686388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <f>'Sales Trends'!B27</f>
-        <v>11635971</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <f>C12/A16</f>
-        <v>5.8988459149648967E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <f>C2/A16</f>
-        <v>9.3077750021893311E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drop na for Quantity and Price in clean script, add revenue data and charts
</commit_message>
<xml_diff>
--- a/data/RetailAnalysis.xlsx
+++ b/data/RetailAnalysis.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Top Customers" sheetId="1" r:id="rId1"/>
     <sheet name="Sales Trends" sheetId="2" r:id="rId2"/>
     <sheet name="Top Ten Products" sheetId="3" r:id="rId3"/>
+    <sheet name="Sales Revenue Trend" sheetId="4" r:id="rId4"/>
+    <sheet name="Top Ten Products By Revenue" sheetId="5" r:id="rId5"/>
+    <sheet name="Top Ten Customers By Revenue" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Ranking</t>
   </si>
@@ -30,9 +33,6 @@
     <t>14646</t>
   </si>
   <si>
-    <t>15152</t>
-  </si>
-  <si>
     <t>13902</t>
   </si>
   <si>
@@ -42,9 +42,6 @@
     <t>13694</t>
   </si>
   <si>
-    <t>15311</t>
-  </si>
-  <si>
     <t>14156</t>
   </si>
   <si>
@@ -57,6 +54,12 @@
     <t>16684</t>
   </si>
   <si>
+    <t>14298</t>
+  </si>
+  <si>
+    <t>12415</t>
+  </si>
+  <si>
     <t>Invoice Date</t>
   </si>
   <si>
@@ -169,6 +172,39 @@
   </si>
   <si>
     <t>PACK OF 72 RETRO SPOT CAKE CASES</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>REGENCY CAKESTAND 3 TIER</t>
+  </si>
+  <si>
+    <t>DOTCOM POSTAGE</t>
+  </si>
+  <si>
+    <t>PARTY BUNTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAPER CHAIN KIT 50'S CHRISTMAS </t>
+  </si>
+  <si>
+    <t>POSTAGE</t>
+  </si>
+  <si>
+    <t>CHILLI LIGHTS</t>
+  </si>
+  <si>
+    <t>ROTATING SILVER ANGELS T-LIGHT HLDR</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>17450</t>
+  </si>
+  <si>
+    <t>15061</t>
   </si>
 </sst>
 </file>
@@ -305,7 +341,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="MonthlySalesRevenue_chart.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="MonthlySales_chart.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -318,7 +354,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3286125" y="190500"/>
+          <a:off x="2600325" y="190500"/>
           <a:ext cx="10972822" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -362,6 +398,135 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4152900" y="190500"/>
+          <a:ext cx="10972822" cy="5486411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152411</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="MonthlySalesRevenue_chart.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3286125" y="190500"/>
+          <a:ext cx="10972822" cy="5486411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152411</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenProductsByRevenue_chart.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4238625" y="190500"/>
+          <a:ext cx="10972822" cy="5486411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152411</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenCustomers_chart.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3200400" y="190500"/>
           <a:ext cx="10972822" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -700,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>281535</v>
+        <v>218090</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -711,7 +876,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>218090</v>
+        <v>186910</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -722,7 +887,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>186910</v>
+        <v>185538</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -733,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>185538</v>
+        <v>163791</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -744,7 +909,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>176000</v>
+        <v>143727</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -755,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>163791</v>
+        <v>117913</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -766,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>143727</v>
+        <v>101095</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -777,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>117913</v>
+        <v>99854</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -788,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>101095</v>
+        <v>91315</v>
       </c>
     </row>
   </sheetData>
@@ -806,7 +971,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -822,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>796632.9400000001</v>
+        <v>444339</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -830,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="1">
-        <v>622354.2120000001</v>
+        <v>395203</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -838,7 +1003,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="1">
-        <v>531206.956</v>
+        <v>391853</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -846,7 +1011,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1">
-        <v>763112.071</v>
+        <v>530301</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -854,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1">
-        <v>587691.032</v>
+        <v>385569</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -862,7 +1027,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="1">
-        <v>613172.53</v>
+        <v>423966</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -870,7 +1035,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1">
-        <v>676873.6899999999</v>
+        <v>413695</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -878,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="1">
-        <v>573146.9300000001</v>
+        <v>358554</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -886,7 +1051,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1">
-        <v>654749.02</v>
+        <v>521757</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -894,7 +1059,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="1">
-        <v>850905.241</v>
+        <v>592590</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -902,7 +1067,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="1">
-        <v>1041505.17</v>
+        <v>622253</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -910,7 +1075,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>1416320.112</v>
+        <v>730369</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -918,7 +1083,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="1">
-        <v>1121929.99</v>
+        <v>542655</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -926,7 +1091,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="1">
-        <v>558368.13</v>
+        <v>397004</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -934,7 +1099,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>496775.03</v>
+        <v>286033</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -942,7 +1107,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="1">
-        <v>681318.05</v>
+        <v>383893</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -950,7 +1115,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="1">
-        <v>491919.041</v>
+        <v>311238</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -958,7 +1123,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="1">
-        <v>720972.25</v>
+        <v>398479</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -966,7 +1131,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="1">
-        <v>689391.15</v>
+        <v>393516</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -974,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="1">
-        <v>678964.781</v>
+        <v>405218</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -982,7 +1147,7 @@
         <v>35</v>
       </c>
       <c r="B22" s="1">
-        <v>681386.46</v>
+        <v>424266</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -990,7 +1155,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="1">
-        <v>1017398.282</v>
+        <v>574063</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -998,7 +1163,7 @@
         <v>37</v>
       </c>
       <c r="B24" s="1">
-        <v>1069265.49</v>
+        <v>626342</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1006,7 +1171,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1">
-        <v>1456089.8</v>
+        <v>768400</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1014,7 +1179,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="1">
-        <v>432699.16</v>
+        <v>314415</v>
       </c>
     </row>
   </sheetData>
@@ -1161,4 +1326,510 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>796632.9400000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>622354.2120000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>531206.956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>763112.071</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1">
+        <v>587691.032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>613172.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>676873.6899999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>573146.9300000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>654749.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>850905.241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1041505.17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1416320.112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1121929.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>558368.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>496775.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1">
+        <v>681318.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1">
+        <v>491919.041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1">
+        <v>720972.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1">
+        <v>689391.15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1">
+        <v>678964.781</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1">
+        <v>681386.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1017398.282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1069265.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1456089.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1">
+        <v>432699.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1">
+        <v>327039.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1">
+        <v>322629.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1">
+        <v>257166.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1">
+        <v>148409.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1">
+        <v>147852.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1">
+        <v>131043.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1">
+        <v>121523.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1">
+        <v>112323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1">
+        <v>84521.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1">
+        <v>73734.28999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>597299.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>523342.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>296378.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>270169.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1">
+        <v>233419.39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>190862.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>171885.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>143269.29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>141502.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1">
+        <v>136341.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
save new charts, update chart tabs and headings
</commit_message>
<xml_diff>
--- a/data/RetailAnalysis.xlsx
+++ b/data/RetailAnalysis.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Top Customers" sheetId="1" r:id="rId1"/>
-    <sheet name="Sales Trends" sheetId="2" r:id="rId2"/>
-    <sheet name="Top Ten Products" sheetId="3" r:id="rId3"/>
+    <sheet name="Top Customers By Quantity" sheetId="1" r:id="rId1"/>
+    <sheet name="Sales Trends By Quantity" sheetId="2" r:id="rId2"/>
+    <sheet name="Top Ten Products By Quantity" sheetId="3" r:id="rId3"/>
     <sheet name="Sales Revenue Trend" sheetId="4" r:id="rId4"/>
     <sheet name="Top Ten Products By Revenue" sheetId="5" r:id="rId5"/>
     <sheet name="Top Ten Customers By Revenue" sheetId="6" r:id="rId6"/>
@@ -211,8 +211,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="$#,##0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -266,12 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +515,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenCustomers_chart.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="TopTenCustomersByRevenue_chart.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1337,7 +1339,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1352,7 +1354,7 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>796632.9400000001</v>
       </c>
     </row>
@@ -1360,7 +1362,7 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>622354.2120000001</v>
       </c>
     </row>
@@ -1368,7 +1370,7 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>531206.956</v>
       </c>
     </row>
@@ -1376,7 +1378,7 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>763112.071</v>
       </c>
     </row>
@@ -1384,7 +1386,7 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>587691.032</v>
       </c>
     </row>
@@ -1392,7 +1394,7 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>613172.53</v>
       </c>
     </row>
@@ -1400,7 +1402,7 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>676873.6899999999</v>
       </c>
     </row>
@@ -1408,7 +1410,7 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>573146.9300000001</v>
       </c>
     </row>
@@ -1416,7 +1418,7 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>654749.02</v>
       </c>
     </row>
@@ -1424,7 +1426,7 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>850905.241</v>
       </c>
     </row>
@@ -1432,7 +1434,7 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>1041505.17</v>
       </c>
     </row>
@@ -1440,7 +1442,7 @@
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>1416320.112</v>
       </c>
     </row>
@@ -1448,7 +1450,7 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>1121929.99</v>
       </c>
     </row>
@@ -1456,7 +1458,7 @@
       <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>558368.13</v>
       </c>
     </row>
@@ -1464,7 +1466,7 @@
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>496775.03</v>
       </c>
     </row>
@@ -1472,7 +1474,7 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>681318.05</v>
       </c>
     </row>
@@ -1480,7 +1482,7 @@
       <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>491919.041</v>
       </c>
     </row>
@@ -1488,7 +1490,7 @@
       <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>720972.25</v>
       </c>
     </row>
@@ -1496,7 +1498,7 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>689391.15</v>
       </c>
     </row>
@@ -1504,7 +1506,7 @@
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>678964.781</v>
       </c>
     </row>
@@ -1512,7 +1514,7 @@
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>681386.46</v>
       </c>
     </row>
@@ -1520,7 +1522,7 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>1017398.282</v>
       </c>
     </row>
@@ -1528,7 +1530,7 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="3">
         <v>1069265.49</v>
       </c>
     </row>
@@ -1536,7 +1538,7 @@
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="3">
         <v>1456089.8</v>
       </c>
     </row>
@@ -1544,7 +1546,7 @@
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>432699.16</v>
       </c>
     </row>
@@ -1564,7 +1566,7 @@
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1585,7 +1587,7 @@
       <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>327039.32</v>
       </c>
     </row>
@@ -1596,7 +1598,7 @@
       <c r="B3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>322629.21</v>
       </c>
     </row>
@@ -1607,7 +1609,7 @@
       <c r="B4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>257166.9</v>
       </c>
     </row>
@@ -1618,7 +1620,7 @@
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>148409.43</v>
       </c>
     </row>
@@ -1629,7 +1631,7 @@
       <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>147852.16</v>
       </c>
     </row>
@@ -1640,7 +1642,7 @@
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>131043.74</v>
       </c>
     </row>
@@ -1651,7 +1653,7 @@
       <c r="B8" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>121523.49</v>
       </c>
     </row>
@@ -1662,7 +1664,7 @@
       <c r="B9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>112323</v>
       </c>
     </row>
@@ -1673,7 +1675,7 @@
       <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>84521.81</v>
       </c>
     </row>
@@ -1684,7 +1686,7 @@
       <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>73734.28999999999</v>
       </c>
     </row>
@@ -1704,7 +1706,7 @@
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1725,7 +1727,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>597299.22</v>
       </c>
     </row>
@@ -1736,7 +1738,7 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>523342.07</v>
       </c>
     </row>
@@ -1747,7 +1749,7 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>296378.14</v>
       </c>
     </row>
@@ -1758,7 +1760,7 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>270169.49</v>
       </c>
     </row>
@@ -1769,7 +1771,7 @@
       <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>233419.39</v>
       </c>
     </row>
@@ -1780,7 +1782,7 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>190862.96</v>
       </c>
     </row>
@@ -1791,7 +1793,7 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>171885.98</v>
       </c>
     </row>
@@ -1802,7 +1804,7 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>143269.29</v>
       </c>
     </row>
@@ -1813,7 +1815,7 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>141502.25</v>
       </c>
     </row>
@@ -1824,7 +1826,7 @@
       <c r="B11" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>136341.48</v>
       </c>
     </row>

</xml_diff>